<commit_message>
Fix: path case or missing file
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -576,154 +576,9 @@
         <v>4/3/2025, 11:37:30 PM</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Ali Abbas sir</v>
-      </c>
-      <c r="C7" t="str">
-        <v>syedazadarhussayn@gmail.com</v>
-      </c>
-      <c r="D7" t="str">
-        <v>09494100110</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Phonics English Course</v>
-      </c>
-      <c r="F7" t="str">
-        <v>79.00</v>
-      </c>
-      <c r="G7" t="str">
-        <v>pay_QEqqXvMyMzckWg</v>
-      </c>
-      <c r="H7" t="str">
-        <v>successful</v>
-      </c>
-      <c r="I7" t="str">
-        <v>4/4/2025, 10:08:53 AM</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Hussain</v>
-      </c>
-      <c r="C8" t="str">
-        <v>syedazadarhussaain998@gmail.com</v>
-      </c>
-      <c r="D8" t="str">
-        <v>9494100110</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Phonics English Course</v>
-      </c>
-      <c r="F8" t="str">
-        <v>79.00</v>
-      </c>
-      <c r="G8" t="str">
-        <v>pay_QEsPGTffT31GDz</v>
-      </c>
-      <c r="H8" t="str">
-        <v>successful</v>
-      </c>
-      <c r="I8" t="str">
-        <v>4/4/2025, 11:40:27 AM</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Ejaz</v>
-      </c>
-      <c r="C9" t="str">
-        <v>syedazadarhussayn12@gmail.com</v>
-      </c>
-      <c r="D9" t="str">
-        <v>9494100110</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Phonics English Course</v>
-      </c>
-      <c r="F9" t="str">
-        <v>79.00</v>
-      </c>
-      <c r="G9" t="str">
-        <v>pay_QEsdvGU92ECHoA</v>
-      </c>
-      <c r="H9" t="str">
-        <v>successful</v>
-      </c>
-      <c r="I9" t="str">
-        <v>4/4/2025, 11:54:20 AM</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Syed Azadar Hussain</v>
-      </c>
-      <c r="C10" t="str">
-        <v>syedazadarhussayn@gmail.com</v>
-      </c>
-      <c r="D10" t="str">
-        <v>09494100110</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Phonics English Course</v>
-      </c>
-      <c r="F10" t="str">
-        <v>79.00</v>
-      </c>
-      <c r="G10" t="str">
-        <v>pay_QEsh9tDttI2qoT</v>
-      </c>
-      <c r="H10" t="str">
-        <v>successful</v>
-      </c>
-      <c r="I10" t="str">
-        <v>4/4/2025, 11:57:23 AM</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="str">
-        <v xml:space="preserve">Syed </v>
-      </c>
-      <c r="C11" t="str">
-        <v>syedazadarhussayn12@gmail.com</v>
-      </c>
-      <c r="D11" t="str">
-        <v>09494100110</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Phonics English Course</v>
-      </c>
-      <c r="F11" t="str">
-        <v>79.00</v>
-      </c>
-      <c r="G11" t="str">
-        <v>pay_QEst9a7ry4dMtq</v>
-      </c>
-      <c r="H11" t="str">
-        <v>successful</v>
-      </c>
-      <c r="I11" t="str">
-        <v>4/4/2025, 12:08:45 PM</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>